<commit_message>
Bug fix in Excel Template
</commit_message>
<xml_diff>
--- a/Software/Zenner Diode Calibration_Data Template.xlsx
+++ b/Software/Zenner Diode Calibration_Data Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aivel\Google Drive (labvelez.share@gmail.com)\Proyect Shares\Lampara IRGA\Calibraciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aivel\source\repos\Curve Fit Example\Curve Fit Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB835FBC-FD0F-4E26-BA6A-DEE1E3CC3D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901D37F8-E690-446D-A8D3-7FACB8B78506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1119,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1164,7 @@
         <v>0.25313482620804456</v>
       </c>
       <c r="D2" s="3">
-        <f>(C2-A2)^2</f>
+        <f t="shared" ref="D2:D32" si="0">(C2-A2)^2</f>
         <v>2.823309756159098E-3</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -1183,11 +1183,11 @@
         <v>0.46454000000000001</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C33" si="0">($I$2-SQRT($I$3-($I$4*B3)))/$I$5</f>
+        <f t="shared" ref="C3:C33" si="1">($I$2-SQRT($I$3-($I$4*B3)))/$I$5</f>
         <v>0.42224247672741172</v>
       </c>
       <c r="D3" s="3">
-        <f>(C3-A3)^2</f>
+        <f t="shared" si="0"/>
         <v>4.9472777096945097E-4</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -1206,11 +1206,11 @@
         <v>0.65485300000000002</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.59456648684933444</v>
       </c>
       <c r="D4" s="3">
-        <f>(C4-A4)^2</f>
+        <f t="shared" si="0"/>
         <v>2.9523065158455327E-5</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -1229,11 +1229,11 @@
         <v>0.84693099999999999</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.77503784192933312</v>
       </c>
       <c r="D5" s="3">
-        <f>(C5-A5)^2</f>
+        <f t="shared" si="0"/>
         <v>6.231093355449621E-4</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1252,11 +1252,11 @@
         <v>1.0323199999999999</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.95621814670795324</v>
       </c>
       <c r="D6" s="3">
-        <f>(C6-A6)^2</f>
+        <f t="shared" si="0"/>
         <v>1.9168506776863054E-3</v>
       </c>
     </row>
@@ -1268,11 +1268,11 @@
         <v>1.2286300000000001</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1565572223382787</v>
       </c>
       <c r="D7" s="3">
-        <f>(C7-A7)^2</f>
+        <f t="shared" si="0"/>
         <v>1.8872749309657444E-3</v>
       </c>
     </row>
@@ -1284,11 +1284,11 @@
         <v>1.41448</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3554253748231537</v>
       </c>
       <c r="D8" s="3">
-        <f>(C8-A8)^2</f>
+        <f t="shared" si="0"/>
         <v>1.9868972096563297E-3</v>
       </c>
     </row>
@@ -1300,11 +1300,11 @@
         <v>1.60318</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5679727742663059</v>
       </c>
       <c r="D9" s="3">
-        <f>(C9-A9)^2</f>
+        <f t="shared" si="0"/>
         <v>1.0257431881970046E-3</v>
       </c>
     </row>
@@ -1316,11 +1316,11 @@
         <v>1.78457</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.784145012994341</v>
       </c>
       <c r="D10" s="3">
-        <f>(C10-A10)^2</f>
+        <f t="shared" si="0"/>
         <v>2.5138061294961624E-4</v>
       </c>
     </row>
@@ -1332,11 +1332,11 @@
         <v>1.9614</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0082399910523958</v>
       </c>
       <c r="D11" s="3">
-        <f>(C11-A11)^2</f>
+        <f t="shared" si="0"/>
         <v>6.7897452543563038E-5</v>
       </c>
     </row>
@@ -1348,11 +1348,11 @@
         <v>2.1280100000000002</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2340046068233197</v>
       </c>
       <c r="D12" s="3">
-        <f>(C12-A12)^2</f>
+        <f t="shared" si="0"/>
         <v>1.1563132852085481E-3</v>
       </c>
     </row>
@@ -1364,11 +1364,11 @@
         <v>2.2417699999999998</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3979936220431717</v>
       </c>
       <c r="D13" s="3">
-        <f>(C13-A13)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0255525056462286E-6</v>
       </c>
     </row>
@@ -1380,11 +1380,11 @@
         <v>2.4181900000000001</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6719574796407093</v>
       </c>
       <c r="D14" s="3">
-        <f>(C14-A14)^2</f>
+        <f t="shared" si="0"/>
         <v>5.1778788762430784E-3</v>
       </c>
     </row>
@@ -1396,11 +1396,11 @@
         <v>2.5383599999999999</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8757456558353591</v>
       </c>
       <c r="D15" s="3">
-        <f>(C15-A15)^2</f>
+        <f t="shared" si="0"/>
         <v>5.7374043779287011E-3</v>
       </c>
     </row>
@@ -1412,11 +1412,11 @@
         <v>2.6438999999999999</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0695705574893584</v>
       </c>
       <c r="D16" s="3">
-        <f>(C16-A16)^2</f>
+        <f t="shared" si="0"/>
         <v>4.8400624693801172E-3</v>
       </c>
     </row>
@@ -1428,11 +1428,11 @@
         <v>2.7375099999999999</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2563126206996031</v>
       </c>
       <c r="D17" s="3">
-        <f>(C17-A17)^2</f>
+        <f t="shared" si="0"/>
         <v>3.1711112500573523E-3</v>
       </c>
     </row>
@@ -1444,11 +1444,11 @@
         <v>2.8192499999999998</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.434056953017631</v>
       </c>
       <c r="D18" s="3">
-        <f>(C18-A18)^2</f>
+        <f t="shared" si="0"/>
         <v>1.1598760488451335E-3</v>
       </c>
     </row>
@@ -1460,11 +1460,11 @@
         <v>2.89242</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.6083184755041131</v>
       </c>
       <c r="D19" s="3">
-        <f>(C19-A19)^2</f>
+        <f t="shared" si="0"/>
         <v>6.9197034712528379E-5</v>
       </c>
       <c r="G19" s="3"/>
@@ -1477,11 +1477,11 @@
         <v>2.92544</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.6928802365164852</v>
       </c>
       <c r="D20" s="3">
-        <f>(C20-A20)^2</f>
+        <f t="shared" si="0"/>
         <v>5.0691032061192954E-5</v>
       </c>
       <c r="G20" s="3"/>
@@ -1494,11 +1494,11 @@
         <v>2.9585499999999998</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7821900301646405</v>
       </c>
       <c r="D21" s="3">
-        <f>(C21-A21)^2</f>
+        <f t="shared" si="0"/>
         <v>3.171950255364088E-4</v>
       </c>
     </row>
@@ -1510,11 +1510,11 @@
         <v>2.9899300000000002</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8717414028175439</v>
       </c>
       <c r="D22" s="3">
-        <f>(C22-A22)^2</f>
+        <f t="shared" si="0"/>
         <v>7.985483147203128E-4</v>
       </c>
     </row>
@@ -1526,11 +1526,11 @@
         <v>3.0185</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.9582076933690322</v>
       </c>
       <c r="D23" s="3">
-        <f>(C23-A23)^2</f>
+        <f t="shared" si="0"/>
         <v>1.7465968935368335E-3</v>
       </c>
     </row>
@@ -1542,11 +1542,11 @@
         <v>3.04644</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0482296524894998</v>
       </c>
       <c r="D24" s="3">
-        <f>(C24-A24)^2</f>
+        <f t="shared" si="0"/>
         <v>2.680168881357913E-3</v>
       </c>
     </row>
@@ -1558,11 +1558,11 @@
         <v>3.0731899999999999</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1405821810255468</v>
       </c>
       <c r="D25" s="3">
-        <f>(C25-A25)^2</f>
+        <f t="shared" si="0"/>
         <v>3.5304772116809165E-3</v>
       </c>
     </row>
@@ -1574,11 +1574,11 @@
         <v>3.0988699999999998</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.2363008996609164</v>
       </c>
       <c r="D26" s="3">
-        <f>(C26-A26)^2</f>
+        <f t="shared" si="0"/>
         <v>4.0575753840086199E-3</v>
       </c>
     </row>
@@ -1590,11 +1590,11 @@
         <v>3.1232700000000002</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3354267481239308</v>
       </c>
       <c r="D27" s="3">
-        <f>(C27-A27)^2</f>
+        <f t="shared" si="0"/>
         <v>4.1697048578503192E-3</v>
       </c>
     </row>
@@ -1606,11 +1606,11 @@
         <v>3.1469200000000002</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4415593857837994</v>
       </c>
       <c r="D28" s="3">
-        <f>(C28-A28)^2</f>
+        <f t="shared" si="0"/>
         <v>3.4153053899667893E-3</v>
       </c>
     </row>
@@ -1622,11 +1622,11 @@
         <v>3.17001</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5584729528833794</v>
       </c>
       <c r="D29" s="3">
-        <f>(C29-A29)^2</f>
+        <f t="shared" si="0"/>
         <v>1.7244956422259984E-3</v>
       </c>
     </row>
@@ -1638,11 +1638,11 @@
         <v>3.1917499999999999</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6866129076537746</v>
       </c>
       <c r="D30" s="3">
-        <f>(C30-A30)^2</f>
+        <f t="shared" si="0"/>
         <v>1.7921424148637186E-4</v>
       </c>
     </row>
@@ -1654,11 +1654,11 @@
         <v>3.2128700000000001</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8400179625840218</v>
       </c>
       <c r="D31" s="3">
-        <f>(C31-A31)^2</f>
+        <f t="shared" si="0"/>
         <v>1.6014373293761861E-3</v>
       </c>
     </row>
@@ -1670,11 +1670,11 @@
         <v>3.2329500000000002</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.0477881960287467</v>
       </c>
       <c r="D32" s="3">
-        <f>(C32-A32)^2</f>
+        <f t="shared" si="0"/>
         <v>2.1841350885431165E-2</v>
       </c>
     </row>
@@ -1685,20 +1685,11 @@
       <c r="B33" s="7">
         <v>3.2524700000000002</v>
       </c>
-      <c r="C33" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="D33" s="3" t="e">
-        <f>(ABS(C33-A33))^2</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="3" t="e">
-        <f>SUM(D2:D33)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>